<commit_message>
Changes done as per meeting held on 17-Apr-2018
</commit_message>
<xml_diff>
--- a/scripts/old_data_migration_to_xml/FilesToRead/MappedExcel_Pune/RHS_Old_New_QuestionMapping_Raghvendra.xlsx
+++ b/scripts/old_data_migration_to_xml/FilesToRead/MappedExcel_Pune/RHS_Old_New_QuestionMapping_Raghvendra.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="539" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="539"/>
   </bookViews>
   <sheets>
     <sheet name="RHSOldNewQuesMapping" sheetId="1" r:id="rId1"/>
     <sheet name="RHSOldNewOptionMapping" sheetId="2" r:id="rId2"/>
     <sheet name="RHSOptionMappingFinal" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" calcOnSave="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="620">
   <si>
     <t>begin_group</t>
   </si>
@@ -1749,42 +1749,18 @@
     <t>Individual</t>
   </si>
   <si>
-    <t>No Service</t>
-  </si>
-  <si>
-    <t>MLA Sponsored Tempo</t>
-  </si>
-  <si>
-    <t>ULB Ghantagadi</t>
-  </si>
-  <si>
-    <t>ULB Van</t>
-  </si>
-  <si>
     <t>Garbage Bin</t>
   </si>
   <si>
     <t>Door to Door Waste Collection</t>
   </si>
   <si>
-    <t>Open Space</t>
-  </si>
-  <si>
     <t>Along/Inside Canal</t>
   </si>
   <si>
     <t>Inside Gutter</t>
   </si>
   <si>
-    <t>Individual toilet</t>
-  </si>
-  <si>
-    <t>Community toilet block (CTB)</t>
-  </si>
-  <si>
-    <t>Public Toilet</t>
-  </si>
-  <si>
     <t>For safety of female family members</t>
   </si>
   <si>
@@ -1794,55 +1770,112 @@
     <t>For any member suffering from illness</t>
   </si>
   <si>
-    <t>Not Applicable</t>
-  </si>
-  <si>
     <t>Satisfied with the CTB</t>
   </si>
   <si>
     <t>Biotoilet</t>
   </si>
   <si>
+    <t xml:space="preserve">Default values to be removed </t>
+  </si>
+  <si>
+    <t>Aadhar Card Number</t>
+  </si>
+  <si>
+    <t>3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>Double House</t>
+  </si>
+  <si>
+    <t>Broken House</t>
+  </si>
+  <si>
+    <t>House Under Construction</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Permanent locked</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Type of toilet Preference (Prefab/Material at door step)</t>
+  </si>
+  <si>
+    <t>4,5,10</t>
+  </si>
+  <si>
+    <t>ULB Ghantagadi/ ULB Van/MLA Sponsored Tempo</t>
+  </si>
+  <si>
+    <t>02,03</t>
+  </si>
+  <si>
+    <t>Tenant/Not giving information</t>
+  </si>
+  <si>
+    <t>02,07</t>
+  </si>
+  <si>
+    <t>Shared connection/Not Giving Information</t>
+  </si>
+  <si>
+    <t>07,1,2</t>
+  </si>
+  <si>
+    <t>Open Space/No Service/Not Giving Information</t>
+  </si>
+  <si>
+    <t>01/"Individual toilet"</t>
+  </si>
+  <si>
+    <t>02/"Community toilet block (CTB)"</t>
+  </si>
+  <si>
+    <t>03/"Shared toilet"</t>
+  </si>
+  <si>
+    <t>06/"Public Toilet"</t>
+  </si>
+  <si>
+    <t>When C3 is 09,10,11,12 then C2 will be 08</t>
+  </si>
+  <si>
+    <t>04/"Open space"</t>
+  </si>
+  <si>
+    <t>Select 02/No for all the records</t>
+  </si>
+  <si>
+    <t>If value for C3 exists then put answer for this else put blank</t>
+  </si>
+  <si>
+    <t>If current place for defication is 04 individual or in combination with other option then set 05/All for this question</t>
+  </si>
+  <si>
+    <t>No/"Not Giving Information"</t>
+  </si>
+  <si>
+    <t>2,3,4,5</t>
+  </si>
+  <si>
+    <t>Brick and cement/Don't know/Not Applicable</t>
+  </si>
+  <si>
+    <t>07,09</t>
+  </si>
+  <si>
+    <t>Non-functional toilet/Not giving information</t>
+  </si>
+  <si>
+    <t>06 option will become blank</t>
+  </si>
+  <si>
     <t>Non-functional toilet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default values to be removed </t>
-  </si>
-  <si>
-    <t>Aadhar Card Number</t>
-  </si>
-  <si>
-    <t>3,4,5,6,7</t>
-  </si>
-  <si>
-    <t>Double House</t>
-  </si>
-  <si>
-    <t>Broken House</t>
-  </si>
-  <si>
-    <t>House Under Construction</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Permanent locked</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Type of toilet Preference (Prefab/Material at door step)</t>
-  </si>
-  <si>
-    <t>Brick and cement</t>
-  </si>
-  <si>
-    <t>Don't know</t>
-  </si>
-  <si>
-    <t>2,3</t>
   </si>
 </sst>
 </file>
@@ -1919,7 +1952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1934,6 +1967,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2240,8 +2274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2312,7 @@
         <v>450</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2483,7 +2517,7 @@
         <v>349</v>
       </c>
       <c r="E16" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="F16">
         <v>549</v>
@@ -2662,6 +2696,9 @@
       <c r="C28" s="8" t="s">
         <v>377</v>
       </c>
+      <c r="D28" s="1" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -2841,6 +2878,9 @@
       <c r="C44" s="3" t="s">
         <v>419</v>
       </c>
+      <c r="D44" s="1" t="s">
+        <v>611</v>
+      </c>
       <c r="E44" t="s">
         <v>566</v>
       </c>
@@ -2859,7 +2899,7 @@
         <v>422</v>
       </c>
       <c r="E45" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="F45">
         <v>455</v>
@@ -2958,6 +2998,9 @@
       </c>
       <c r="C52" s="8" t="s">
         <v>441</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3467,10 +3510,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O294"/>
+  <dimension ref="A1:O291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B144" workbookViewId="0">
-      <selection activeCell="J244" sqref="J244"/>
+    <sheetView topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="D212" sqref="D212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5249,7 +5292,7 @@
         <v>440</v>
       </c>
       <c r="J127" s="6" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.25">
@@ -5301,7 +5344,7 @@
         <v>498</v>
       </c>
       <c r="K130" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
     </row>
     <row r="131" spans="2:11" x14ac:dyDescent="0.25">
@@ -5324,7 +5367,7 @@
         <v>512</v>
       </c>
       <c r="K131" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.25">
@@ -5347,7 +5390,7 @@
         <v>513</v>
       </c>
       <c r="K132" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.25">
@@ -5367,10 +5410,10 @@
         <v>440</v>
       </c>
       <c r="J133" s="6" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
       <c r="K133" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
     </row>
     <row r="134" spans="2:11" x14ac:dyDescent="0.25">
@@ -5390,7 +5433,7 @@
         <v>440</v>
       </c>
       <c r="J134" s="6" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
       <c r="K134" t="s">
         <v>573</v>
@@ -5597,25 +5640,21 @@
         <v>557</v>
       </c>
       <c r="J147" s="6" t="s">
-        <v>141</v>
+        <v>598</v>
       </c>
       <c r="K147" s="6" t="s">
-        <v>278</v>
+        <v>599</v>
       </c>
     </row>
     <row r="148" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B148" s="3" t="s">
+        <v>477</v>
+      </c>
       <c r="C148" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="H148" t="s">
-        <v>557</v>
-      </c>
-      <c r="I148">
-        <v>557</v>
-      </c>
-      <c r="K148" s="6" t="s">
-        <v>291</v>
-      </c>
+      <c r="D148" s="6"/>
+      <c r="K148" s="6"/>
     </row>
     <row r="149" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J149" s="7"/>
@@ -5751,10 +5790,10 @@
         <v>411</v>
       </c>
       <c r="J157" s="6" t="s">
-        <v>141</v>
+        <v>600</v>
       </c>
       <c r="K157" s="6" t="s">
-        <v>293</v>
+        <v>601</v>
       </c>
     </row>
     <row r="158" spans="2:11" x14ac:dyDescent="0.25">
@@ -5826,7 +5865,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
         <v>484</v>
       </c>
@@ -5849,7 +5888,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="162" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="10"/>
       <c r="B162" s="8" t="s">
         <v>484</v>
@@ -5861,57 +5900,33 @@
         <v>487</v>
       </c>
       <c r="G162" s="12"/>
-      <c r="H162" s="11" t="s">
-        <v>559</v>
-      </c>
-      <c r="I162" s="11">
-        <v>411</v>
-      </c>
-      <c r="J162" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="K162" s="13" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="5"/>
-      <c r="C163" s="5"/>
-      <c r="D163" s="5"/>
-      <c r="J163" s="7"/>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B164" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="H164" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="I164" s="11">
-        <v>439</v>
-      </c>
-      <c r="J164" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="K164" s="13" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J162" s="13"/>
+      <c r="K162" s="13"/>
+    </row>
+    <row r="163" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="10"/>
+      <c r="B163" s="8"/>
+      <c r="C163" s="8"/>
+      <c r="D163" s="8"/>
+      <c r="G163" s="12"/>
+      <c r="J163" s="13"/>
+      <c r="K163" s="13"/>
+    </row>
+    <row r="164" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="5"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="J164" s="7"/>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
         <v>488</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H165" s="11" t="s">
         <v>570</v>
@@ -5919,45 +5934,49 @@
       <c r="I165" s="11">
         <v>439</v>
       </c>
-      <c r="J165" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="K165" s="13" t="s">
+      <c r="J165" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K165" s="6" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L165" s="13"/>
+      <c r="M165" s="13"/>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
         <v>488</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H166" t="s">
+        <v>297</v>
+      </c>
+      <c r="H166" s="11" t="s">
         <v>570</v>
       </c>
-      <c r="I166">
+      <c r="I166" s="11">
         <v>439</v>
       </c>
       <c r="J166" s="6" t="s">
-        <v>143</v>
+        <v>596</v>
       </c>
       <c r="K166" s="6" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+        <v>597</v>
+      </c>
+      <c r="L166" s="13"/>
+      <c r="M166" s="13"/>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
         <v>488</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H167" t="s">
         <v>570</v>
@@ -5966,21 +5985,23 @@
         <v>439</v>
       </c>
       <c r="J167" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K167" s="6" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+      <c r="L167" s="6"/>
+      <c r="M167" s="6"/>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
         <v>488</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H168" t="s">
         <v>570</v>
@@ -5989,21 +6010,23 @@
         <v>439</v>
       </c>
       <c r="J168" s="6" t="s">
-        <v>145</v>
+        <v>602</v>
       </c>
       <c r="K168" s="6" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="L168" s="6"/>
+      <c r="M168" s="6"/>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
         <v>488</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H169" t="s">
         <v>570</v>
@@ -6012,13 +6035,22 @@
         <v>439</v>
       </c>
       <c r="J169" s="6" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="K169" s="6" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B170" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="H170" t="s">
         <v>570</v>
       </c>
@@ -6026,77 +6058,63 @@
         <v>439</v>
       </c>
       <c r="J170" s="6" t="s">
-        <v>146</v>
+        <v>516</v>
       </c>
       <c r="K170" s="6" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H171" t="s">
-        <v>570</v>
-      </c>
-      <c r="I171">
-        <v>439</v>
-      </c>
-      <c r="J171" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="K171" s="6" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H172" t="s">
-        <v>570</v>
-      </c>
-      <c r="I172">
-        <v>439</v>
-      </c>
-      <c r="J172" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="K172" s="6" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H173" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="I173" s="11">
-        <v>439</v>
-      </c>
-      <c r="J173" s="13" t="s">
-        <v>518</v>
-      </c>
-      <c r="K173" s="13" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J174" s="7"/>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H171" s="11"/>
+      <c r="I171" s="11"/>
+      <c r="L171" s="13"/>
+      <c r="M171" s="13"/>
+    </row>
+    <row r="172" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J172" s="7"/>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B173" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B174" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
         <v>489</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
         <v>489</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="177" spans="2:10" x14ac:dyDescent="0.25">
@@ -6104,77 +6122,77 @@
         <v>489</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="178" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B178" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>323</v>
-      </c>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="178" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B178" s="5"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="5"/>
+      <c r="J178" s="7"/>
     </row>
     <row r="179" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B179" s="3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="180" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B180" s="5"/>
-      <c r="C180" s="5"/>
-      <c r="D180" s="5"/>
-      <c r="J180" s="7"/>
-    </row>
-    <row r="181" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B181" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="180" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B180" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="C181" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>279</v>
-      </c>
+      <c r="C180" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="181" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="5"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="5"/>
+      <c r="J181" s="7"/>
     </row>
     <row r="182" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B182" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C182" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="183" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B183" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C183" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D182" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="183" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B183" s="5"/>
-      <c r="C183" s="5"/>
-      <c r="D183" s="5"/>
-      <c r="J183" s="7"/>
+      <c r="D183" s="3" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="184" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
         <v>492</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="185" spans="2:10" x14ac:dyDescent="0.25">
@@ -6182,49 +6200,49 @@
         <v>492</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="186" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B186" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>495</v>
-      </c>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="186" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B186" s="5"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+      <c r="J186" s="7"/>
     </row>
     <row r="187" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B187" s="3" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="188" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="5"/>
-      <c r="C188" s="5"/>
-      <c r="D188" s="5"/>
-      <c r="J188" s="7"/>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="188" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B188" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="189" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
         <v>497</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="190" spans="2:10" x14ac:dyDescent="0.25">
@@ -6232,366 +6250,399 @@
         <v>497</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="191" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B191" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D191" s="3" t="s">
-        <v>317</v>
-      </c>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="191" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B191" s="5"/>
+      <c r="C191" s="5"/>
+      <c r="D191" s="5"/>
+      <c r="J191" s="7"/>
     </row>
     <row r="192" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="193" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="5"/>
-      <c r="C193" s="5"/>
-      <c r="D193" s="5"/>
-      <c r="J193" s="7"/>
-    </row>
-    <row r="194" spans="2:10" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B193" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
         <v>499</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="195" spans="2:10" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
         <v>499</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="196" spans="2:10" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
         <v>499</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="197" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B197" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="198" spans="2:10" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B197" s="5"/>
+      <c r="C197" s="5"/>
+      <c r="D197" s="5"/>
+      <c r="J197" s="7"/>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="199" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="5"/>
-      <c r="C199" s="5"/>
-      <c r="D199" s="5"/>
-      <c r="J199" s="7"/>
-    </row>
-    <row r="200" spans="2:10" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B199" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
         <v>503</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="201" spans="2:10" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
         <v>503</v>
       </c>
       <c r="C201" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B202" s="5"/>
+      <c r="C202" s="5"/>
+      <c r="D202" s="5"/>
+      <c r="J202" s="7"/>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B204" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C204" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D201" s="3" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="202" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B202" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D202" s="3" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="203" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B203" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="C203" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D203" s="3" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="204" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="5"/>
-      <c r="C204" s="5"/>
-      <c r="D204" s="5"/>
-      <c r="J204" s="7"/>
-    </row>
-    <row r="205" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D204" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
         <v>508</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="206" spans="2:10" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
         <v>508</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="207" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B207" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D207" s="3" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="208" spans="2:10" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B207" s="5"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+      <c r="J207" s="7"/>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="B208" s="3" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="209" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B209" s="5"/>
-      <c r="C209" s="5"/>
-      <c r="D209" s="5"/>
-      <c r="J209" s="7"/>
-    </row>
-    <row r="210" spans="2:10" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="G208" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B209" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="F209" s="3" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
         <v>511</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="211" spans="2:10" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+      <c r="F210" s="3" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
         <v>511</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="F211" s="3" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="212" spans="2:10" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+      <c r="G211" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="C212" s="3" t="s">
-        <v>146</v>
+      <c r="C212" s="14">
+        <v>13</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="F212" s="3" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="213" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B213" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D213" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="214" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B214" s="5"/>
-      <c r="C214" s="5"/>
-      <c r="D214" s="5"/>
-      <c r="J214" s="7"/>
-    </row>
-    <row r="215" spans="2:10" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B213" s="5"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="5"/>
+      <c r="J213" s="7"/>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="G214" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
         <v>515</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="216" spans="2:10" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="G215" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B216" s="3" t="s">
         <v>515</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="217" spans="2:10" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+      <c r="G216" s="2" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B217" s="3" t="s">
         <v>515</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="218" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B218" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="D218" s="3" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="219" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B219" s="5"/>
-      <c r="C219" s="5"/>
-      <c r="D219" s="5"/>
-      <c r="J219" s="7"/>
-    </row>
-    <row r="220" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G217" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B218" s="5"/>
+      <c r="C218" s="5"/>
+      <c r="D218" s="5"/>
+      <c r="J218" s="7"/>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
         <v>521</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="221" spans="2:10" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
         <v>521</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="222" spans="2:10" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
         <v>521</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="223" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B223" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="D223" s="3" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="224" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="5"/>
-      <c r="C224" s="5"/>
-      <c r="D224" s="5"/>
-      <c r="J224" s="7"/>
+    <row r="223" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B223" s="5"/>
+      <c r="C223" s="5"/>
+      <c r="D223" s="5"/>
+      <c r="J223" s="7"/>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="225" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
         <v>522</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>517</v>
+        <v>282</v>
       </c>
     </row>
     <row r="226" spans="2:11" x14ac:dyDescent="0.25">
@@ -6599,10 +6650,10 @@
         <v>522</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="227" spans="2:11" x14ac:dyDescent="0.25">
@@ -6610,328 +6661,323 @@
         <v>522</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="228" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B228" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="C228" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="D228" s="3" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="229" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="5"/>
-      <c r="C229" s="5"/>
-      <c r="D229" s="5"/>
-      <c r="J229" s="7"/>
+    <row r="228" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B228" s="5"/>
+      <c r="C228" s="5"/>
+      <c r="D228" s="5"/>
+      <c r="J228" s="7"/>
+    </row>
+    <row r="229" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B229" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="K229" s="6"/>
     </row>
     <row r="230" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
         <v>523</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="H230" t="s">
-        <v>565</v>
-      </c>
-      <c r="I230">
-        <v>558</v>
-      </c>
-      <c r="J230" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K230" s="6" t="s">
-        <v>586</v>
-      </c>
+        <v>525</v>
+      </c>
+      <c r="K230" s="6"/>
     </row>
     <row r="231" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
         <v>523</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="H231" t="s">
-        <v>565</v>
-      </c>
-      <c r="I231">
-        <v>558</v>
-      </c>
-      <c r="J231" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K231" s="6" t="s">
-        <v>587</v>
-      </c>
+        <v>526</v>
+      </c>
+      <c r="K231" s="6"/>
     </row>
     <row r="232" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
         <v>523</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="H232" t="s">
-        <v>565</v>
-      </c>
-      <c r="I232">
-        <v>558</v>
-      </c>
-      <c r="J232" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K232" s="6" t="s">
-        <v>282</v>
-      </c>
+        <v>527</v>
+      </c>
+      <c r="K232" s="6"/>
     </row>
     <row r="233" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B233" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="C233" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D233" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="H233" t="s">
-        <v>565</v>
-      </c>
-      <c r="I233">
-        <v>558</v>
-      </c>
-      <c r="J233" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="K233" s="6" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="234" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J234" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="K234" s="6" t="s">
-        <v>291</v>
-      </c>
+      <c r="K233" s="6"/>
+    </row>
+    <row r="234" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J234" s="7"/>
     </row>
     <row r="235" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B235" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H235" t="s">
+        <v>566</v>
+      </c>
+      <c r="I235">
+        <v>441</v>
+      </c>
+      <c r="J235" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="K235" s="6" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="236" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J236" s="7"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="236" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B236" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="G236" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="H236" t="s">
+        <v>566</v>
+      </c>
+      <c r="I236">
+        <v>441</v>
+      </c>
+      <c r="J236" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="K236" s="6" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="237" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B237" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="C237" s="3" t="s">
+      <c r="B237" s="3"/>
+      <c r="C237" s="3"/>
+      <c r="D237" s="3"/>
+      <c r="K237" s="6"/>
+    </row>
+    <row r="238" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B238" s="5"/>
+      <c r="C238" s="5"/>
+      <c r="D238" s="5"/>
+      <c r="J238" s="7"/>
+    </row>
+    <row r="239" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B239" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="C239" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D237" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="H237" t="s">
-        <v>566</v>
-      </c>
-      <c r="I237">
-        <v>441</v>
-      </c>
-      <c r="J237" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K237" s="6" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="238" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B238" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="C238" s="3" t="s">
+      <c r="D239" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="H239" t="s">
+        <v>595</v>
+      </c>
+      <c r="I239">
+        <v>455</v>
+      </c>
+      <c r="J239" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="K239" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="240" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B240" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="C240" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D238" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="H238" t="s">
-        <v>566</v>
-      </c>
-      <c r="I238">
-        <v>441</v>
-      </c>
-      <c r="J238" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K238" s="6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="239" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B239" s="3"/>
-      <c r="C239" s="3"/>
-      <c r="D239" s="3"/>
-      <c r="H239" t="s">
-        <v>566</v>
-      </c>
-      <c r="I239">
-        <v>441</v>
-      </c>
-      <c r="K239" s="6" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="240" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B240" s="3"/>
-      <c r="C240" s="3"/>
-      <c r="D240" s="3"/>
+      <c r="D240" s="3" t="s">
+        <v>530</v>
+      </c>
       <c r="H240" t="s">
-        <v>566</v>
+        <v>595</v>
       </c>
       <c r="I240">
-        <v>441</v>
-      </c>
-      <c r="K240" s="6" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="241" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="5"/>
-      <c r="C241" s="5"/>
-      <c r="D241" s="5"/>
-      <c r="J241" s="7"/>
-    </row>
-    <row r="242" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B242" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="C242" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D242" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H242" t="s">
-        <v>605</v>
-      </c>
-      <c r="I242">
         <v>455</v>
       </c>
-      <c r="J242" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="K242" t="s">
-        <v>314</v>
-      </c>
-    </row>
+      <c r="J240" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="K240" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="241" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J241"/>
+    </row>
+    <row r="242" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="243" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C243" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="244" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B244" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="C244" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D243" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="H243" t="s">
-        <v>605</v>
-      </c>
-      <c r="I243">
-        <v>455</v>
-      </c>
-      <c r="J243" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="K243" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="244" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J244" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="K244" t="s">
-        <v>607</v>
+      <c r="D244" s="3" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="245" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J245" t="s">
-        <v>144</v>
-      </c>
-      <c r="K245" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="246" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B245" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="246" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B246" s="5"/>
+      <c r="C246" s="5"/>
+      <c r="D246" s="5"/>
+      <c r="J246" s="7"/>
+    </row>
     <row r="247" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>493</v>
+        <v>534</v>
+      </c>
+      <c r="H247" t="s">
+        <v>567</v>
+      </c>
+      <c r="I247">
+        <v>443</v>
+      </c>
+      <c r="J247" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K247" s="6" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="248" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>494</v>
+        <v>535</v>
+      </c>
+      <c r="H248" t="s">
+        <v>567</v>
+      </c>
+      <c r="I248">
+        <v>443</v>
+      </c>
+      <c r="J248" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K248" s="6" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="249" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>142</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="250" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="5"/>
-      <c r="C250" s="5"/>
-      <c r="D250" s="5"/>
-      <c r="J250" s="7"/>
+        <v>302</v>
+      </c>
+      <c r="H249" t="s">
+        <v>567</v>
+      </c>
+      <c r="I249">
+        <v>443</v>
+      </c>
+      <c r="J249" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K249" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="250" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B250" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="C250" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D250" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H250" t="s">
+        <v>567</v>
+      </c>
+      <c r="I250">
+        <v>443</v>
+      </c>
+      <c r="J250" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="K250" s="6" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="251" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B251" s="3" t="s">
         <v>533</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>534</v>
+        <v>304</v>
       </c>
       <c r="H251" t="s">
         <v>567</v>
@@ -6940,10 +6986,10 @@
         <v>443</v>
       </c>
       <c r="J251" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K251" s="6" t="s">
-        <v>589</v>
+        <v>304</v>
       </c>
     </row>
     <row r="252" spans="2:11" x14ac:dyDescent="0.25">
@@ -6951,10 +6997,10 @@
         <v>533</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>535</v>
+        <v>305</v>
       </c>
       <c r="H252" t="s">
         <v>567</v>
@@ -6963,10 +7009,10 @@
         <v>443</v>
       </c>
       <c r="J252" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K252" s="6" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
     </row>
     <row r="253" spans="2:11" x14ac:dyDescent="0.25">
@@ -6974,10 +7020,10 @@
         <v>533</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="H253" t="s">
         <v>567</v>
@@ -6986,10 +7032,10 @@
         <v>443</v>
       </c>
       <c r="J253" s="6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="K253" s="6" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="254" spans="2:11" x14ac:dyDescent="0.25">
@@ -6997,10 +7043,10 @@
         <v>533</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="H254" t="s">
         <v>567</v>
@@ -7009,130 +7055,119 @@
         <v>443</v>
       </c>
       <c r="J254" s="6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K254" s="6" t="s">
-        <v>303</v>
+        <v>324</v>
       </c>
     </row>
     <row r="255" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B255" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="C255" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D255" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="H255" t="s">
-        <v>567</v>
-      </c>
-      <c r="I255">
-        <v>443</v>
-      </c>
-      <c r="J255" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="K255" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="256" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B256" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="C256" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D256" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="H256" t="s">
-        <v>567</v>
-      </c>
-      <c r="I256">
-        <v>443</v>
-      </c>
-      <c r="J256" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K256" s="6" t="s">
-        <v>591</v>
-      </c>
+      <c r="K255" s="6"/>
+    </row>
+    <row r="256" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J256" s="7"/>
     </row>
     <row r="257" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B257" s="3" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="H257" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="I257">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J257" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K257" s="6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="258" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B258" s="3" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H258" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="I258">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J258" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K258" s="6" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="259" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B259" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C259" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D259" s="3" t="s">
+        <v>310</v>
+      </c>
       <c r="H259" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="I259">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J259" s="6" t="s">
-        <v>516</v>
+        <v>142</v>
       </c>
       <c r="K259" s="6" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="260" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J260" s="7"/>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="260" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B260" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D260" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="H260" t="s">
+        <v>568</v>
+      </c>
+      <c r="I260">
+        <v>442</v>
+      </c>
+      <c r="J260" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="K260" s="6" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="261" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B261" s="3" t="s">
         <v>536</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>308</v>
+        <v>537</v>
       </c>
       <c r="H261" t="s">
         <v>568</v>
@@ -7141,10 +7176,10 @@
         <v>442</v>
       </c>
       <c r="J261" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K261" s="6" t="s">
-        <v>308</v>
+        <v>584</v>
       </c>
     </row>
     <row r="262" spans="2:11" x14ac:dyDescent="0.25">
@@ -7152,10 +7187,10 @@
         <v>536</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="H262" t="s">
         <v>568</v>
@@ -7164,10 +7199,10 @@
         <v>442</v>
       </c>
       <c r="J262" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K262" s="6" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="263" spans="2:11" x14ac:dyDescent="0.25">
@@ -7175,10 +7210,10 @@
         <v>536</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="H263" t="s">
         <v>568</v>
@@ -7187,10 +7222,10 @@
         <v>442</v>
       </c>
       <c r="J263" s="6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="K263" s="6" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="264" spans="2:11" x14ac:dyDescent="0.25">
@@ -7198,10 +7233,10 @@
         <v>536</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H264" t="s">
         <v>568</v>
@@ -7210,130 +7245,119 @@
         <v>442</v>
       </c>
       <c r="J264" s="6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K264" s="6" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="265" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B265" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="C265" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D265" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="H265" t="s">
-        <v>568</v>
-      </c>
-      <c r="I265">
-        <v>442</v>
-      </c>
-      <c r="J265" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="K265" s="6" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="266" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B266" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="C266" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D266" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="H266" t="s">
-        <v>568</v>
-      </c>
-      <c r="I266">
-        <v>442</v>
-      </c>
-      <c r="J266" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K266" s="6" t="s">
-        <v>312</v>
-      </c>
+      <c r="K265" s="6"/>
+    </row>
+    <row r="266" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J266" s="7"/>
     </row>
     <row r="267" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B267" s="3" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
       <c r="H267" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="I267">
-        <v>442</v>
+        <v>555</v>
       </c>
       <c r="J267" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K267" s="6" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
     </row>
     <row r="268" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B268" s="3" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="H268" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="I268">
-        <v>442</v>
+        <v>555</v>
       </c>
       <c r="J268" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K268" s="6" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
     </row>
     <row r="269" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B269" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>289</v>
+      </c>
       <c r="H269" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="I269">
-        <v>442</v>
+        <v>555</v>
       </c>
       <c r="J269" s="6" t="s">
-        <v>516</v>
+        <v>142</v>
       </c>
       <c r="K269" s="6" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="270" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J270" s="7"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="270" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B270" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="C270" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D270" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="H270" t="s">
+        <v>569</v>
+      </c>
+      <c r="I270">
+        <v>555</v>
+      </c>
+      <c r="J270" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="K270" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="271" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B271" s="3" t="s">
         <v>538</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>287</v>
+        <v>539</v>
       </c>
       <c r="H271" t="s">
         <v>569</v>
@@ -7342,10 +7366,10 @@
         <v>555</v>
       </c>
       <c r="J271" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K271" s="6" t="s">
-        <v>287</v>
+        <v>539</v>
       </c>
     </row>
     <row r="272" spans="2:11" x14ac:dyDescent="0.25">
@@ -7353,10 +7377,10 @@
         <v>538</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>288</v>
+        <v>540</v>
       </c>
       <c r="H272" t="s">
         <v>569</v>
@@ -7365,10 +7389,10 @@
         <v>555</v>
       </c>
       <c r="J272" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K272" s="6" t="s">
-        <v>288</v>
+        <v>585</v>
       </c>
     </row>
     <row r="273" spans="2:11" x14ac:dyDescent="0.25">
@@ -7376,10 +7400,10 @@
         <v>538</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>289</v>
+        <v>541</v>
       </c>
       <c r="H273" t="s">
         <v>569</v>
@@ -7387,22 +7411,17 @@
       <c r="I273">
         <v>555</v>
       </c>
-      <c r="J273" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K273" s="6" t="s">
-        <v>289</v>
-      </c>
+      <c r="K273" s="7"/>
     </row>
     <row r="274" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B274" s="3" t="s">
         <v>538</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H274" t="s">
         <v>569</v>
@@ -7411,21 +7430,18 @@
         <v>555</v>
       </c>
       <c r="J274" s="6" t="s">
-        <v>143</v>
+        <v>616</v>
       </c>
       <c r="K274" s="6" t="s">
-        <v>290</v>
+        <v>617</v>
       </c>
     </row>
     <row r="275" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B275" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="C275" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D275" s="3" t="s">
-        <v>539</v>
+      <c r="C275" s="14" t="s">
+        <v>516</v>
       </c>
       <c r="H275" t="s">
         <v>569</v>
@@ -7434,135 +7450,90 @@
         <v>555</v>
       </c>
       <c r="J275" s="6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="K275" s="6" t="s">
-        <v>539</v>
+        <v>574</v>
       </c>
     </row>
     <row r="276" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B276" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="C276" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D276" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="H276" t="s">
-        <v>569</v>
-      </c>
-      <c r="I276">
-        <v>555</v>
-      </c>
-      <c r="J276" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K276" s="6" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="277" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B277" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="C277" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D277" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="H277" t="s">
-        <v>569</v>
-      </c>
-      <c r="I277">
-        <v>555</v>
-      </c>
-      <c r="J277" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="K277" s="7" t="s">
-        <v>595</v>
-      </c>
+      <c r="B276" s="3"/>
+      <c r="C276" s="14"/>
+      <c r="K276" s="6"/>
+    </row>
+    <row r="277" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J277" s="7"/>
     </row>
     <row r="278" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B278" s="3" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="H278" t="s">
-        <v>569</v>
-      </c>
-      <c r="I278">
-        <v>555</v>
-      </c>
-      <c r="J278" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="K278" s="6" t="s">
-        <v>291</v>
+        <v>543</v>
       </c>
     </row>
     <row r="279" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H279" t="s">
-        <v>569</v>
-      </c>
-      <c r="I279">
-        <v>555</v>
-      </c>
-      <c r="J279" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="K279" s="6" t="s">
-        <v>574</v>
+      <c r="B279" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="C279" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D279" s="3" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="280" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B280" s="5"/>
+      <c r="C280" s="5"/>
+      <c r="D280" s="5"/>
       <c r="J280" s="7"/>
     </row>
     <row r="281" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B281" s="3" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C281" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="282" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B282" s="3" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="283" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B283" s="5"/>
-      <c r="C283" s="5"/>
-      <c r="D283" s="5"/>
-      <c r="J283" s="7"/>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="283" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B283" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C283" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D283" s="3" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="284" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B284" s="3" t="s">
         <v>545</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="285" spans="2:11" x14ac:dyDescent="0.25">
@@ -7570,115 +7541,82 @@
         <v>545</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="286" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B286" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="C286" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D286" s="3" t="s">
-        <v>548</v>
-      </c>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="286" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B286" s="5"/>
+      <c r="C286" s="5"/>
+      <c r="D286" s="5"/>
+      <c r="J286" s="7"/>
     </row>
     <row r="287" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B287" s="3" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>549</v>
+        <v>284</v>
       </c>
     </row>
     <row r="288" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B288" s="3" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="C288" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="289" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B289" s="5"/>
-      <c r="C289" s="5"/>
-      <c r="D289" s="5"/>
-      <c r="J289" s="7"/>
-    </row>
-    <row r="290" spans="2:10" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+      <c r="F288" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="289" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B289" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="F289" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="290" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B290" s="3" t="s">
         <v>550</v>
       </c>
       <c r="C290" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D290" s="3" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="291" spans="2:10" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="F290" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="291" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B291" s="3" t="s">
         <v>550</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D291" s="3" t="s">
-        <v>551</v>
+        <v>286</v>
       </c>
       <c r="F291" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="292" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B292" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="C292" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D292" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="F292" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="293" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B293" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="C293" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D293" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="F293" s="3" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="294" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B294" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="C294" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D294" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="F294" s="3" t="s">
         <v>512</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added changes to read the data from excel file for generating the xml to be uploaded to KOBO server for PMC RHS. Also added change in the upload file script to move the file to another location once the file is uploaded to have a track of which files have been processed and which are yet to be processed. Currently the script for PHS will fetch the data from the excel and not from database.
</commit_message>
<xml_diff>
--- a/scripts/old_data_migration_to_xml/FilesToRead/MappedExcel_Pune/RHS_Old_New_QuestionMapping_Raghvendra.xlsx
+++ b/scripts/old_data_migration_to_xml/FilesToRead/MappedExcel_Pune/RHS_Old_New_QuestionMapping_Raghvendra.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="539"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="539" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RHSOldNewQuesMapping" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="630">
   <si>
     <t>begin_group</t>
   </si>
@@ -1740,9 +1740,6 @@
     <t>Not Giving Information</t>
   </si>
   <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
     <t>Water stand-posts</t>
   </si>
   <si>
@@ -1866,23 +1863,56 @@
     <t>Brick and cement/Don't know/Not Applicable</t>
   </si>
   <si>
-    <t>07,09</t>
-  </si>
-  <si>
-    <t>Non-functional toilet/Not giving information</t>
-  </si>
-  <si>
     <t>06 option will become blank</t>
   </si>
   <si>
     <t>Non-functional toilet</t>
+  </si>
+  <si>
+    <t>DataExcelQuestionSequenceNumber</t>
+  </si>
+  <si>
+    <t>Non-functional toilet/Not giving information/Not applicable</t>
+  </si>
+  <si>
+    <t>07,09,08</t>
+  </si>
+  <si>
+    <t>08,09</t>
+  </si>
+  <si>
+    <t>Lohagaon Viman Nagar, Yamuna Nagar Pune S.N.199</t>
+  </si>
+  <si>
+    <t>SanjayPark Zopadpatti</t>
+  </si>
+  <si>
+    <t>Ambedkar Vasahat, D.P.Road, Aundh, S.N. 159/160</t>
+  </si>
+  <si>
+    <t>Sangamwadi Kachi Vasti 1</t>
+  </si>
+  <si>
+    <t>Sanjay Gandhi Vasahat Karve Nagar S.N. 39/2</t>
+  </si>
+  <si>
+    <t>Mahatma Phule/Savitribai Phule, Parvati</t>
+  </si>
+  <si>
+    <t>Gosavi Vasti, Dhayri Phata</t>
+  </si>
+  <si>
+    <t>Panmala, Parvati</t>
+  </si>
+  <si>
+    <t>S.N. 85 Ambedkar Nagar, Sahakar Nagar No. 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1911,6 +1941,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1952,7 +1988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1968,6 +2004,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2274,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,11 +2349,14 @@
       <c r="F1" t="s">
         <v>449</v>
       </c>
+      <c r="G1" t="s">
+        <v>617</v>
+      </c>
       <c r="H1" t="s">
         <v>450</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2387,6 +2431,9 @@
       <c r="F6">
         <v>416</v>
       </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2403,6 +2450,9 @@
       </c>
       <c r="F7">
         <v>440</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2419,6 +2469,9 @@
       <c r="F8">
         <v>440</v>
       </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -2458,6 +2511,9 @@
       <c r="F11">
         <v>222</v>
       </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2505,6 +2561,9 @@
       <c r="F15">
         <v>550</v>
       </c>
+      <c r="G15">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -2517,13 +2576,16 @@
         <v>349</v>
       </c>
       <c r="E16" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F16">
         <v>549</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -2539,8 +2601,11 @@
       <c r="F17">
         <v>415</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>352</v>
       </c>
@@ -2556,8 +2621,11 @@
       <c r="F18">
         <v>559</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -2573,8 +2641,11 @@
       <c r="F19">
         <v>560</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>357</v>
       </c>
@@ -2590,8 +2661,11 @@
       <c r="F20">
         <v>556</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>359</v>
       </c>
@@ -2607,8 +2681,11 @@
       <c r="F21">
         <v>557</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>362</v>
       </c>
@@ -2624,8 +2701,11 @@
       <c r="F22">
         <v>410</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>365</v>
       </c>
@@ -2641,8 +2721,11 @@
       <c r="F23">
         <v>411</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>367</v>
       </c>
@@ -2658,8 +2741,11 @@
       <c r="F24">
         <v>439</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>370</v>
       </c>
@@ -2670,12 +2756,12 @@
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>0</v>
       </c>
@@ -2686,7 +2772,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>375</v>
       </c>
@@ -2697,10 +2783,10 @@
         <v>377</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>378</v>
       </c>
@@ -2711,7 +2797,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>381</v>
       </c>
@@ -2722,7 +2808,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>5</v>
       </c>
@@ -2733,7 +2819,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>5</v>
       </c>
@@ -2744,7 +2830,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>5</v>
       </c>
@@ -2755,7 +2841,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>390</v>
       </c>
@@ -2766,7 +2852,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>393</v>
       </c>
@@ -2777,7 +2863,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2788,7 +2874,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>398</v>
       </c>
@@ -2799,7 +2885,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>401</v>
       </c>
@@ -2810,7 +2896,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>404</v>
       </c>
@@ -2821,7 +2907,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>407</v>
       </c>
@@ -2832,7 +2918,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>410</v>
       </c>
@@ -2843,7 +2929,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>14</v>
       </c>
@@ -2856,8 +2942,11 @@
       <c r="F42">
         <v>558</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>414</v>
       </c>
@@ -2868,7 +2957,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>417</v>
       </c>
@@ -2879,7 +2968,7 @@
         <v>419</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E44" t="s">
         <v>566</v>
@@ -2887,8 +2976,11 @@
       <c r="F44">
         <v>441</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>420</v>
       </c>
@@ -2899,13 +2991,16 @@
         <v>422</v>
       </c>
       <c r="E45" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F45">
         <v>455</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>423</v>
       </c>
@@ -2916,7 +3011,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>426</v>
       </c>
@@ -2932,8 +3027,11 @@
       <c r="F47">
         <v>443</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>428</v>
       </c>
@@ -2949,8 +3047,11 @@
       <c r="F48">
         <v>442</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>430</v>
       </c>
@@ -2966,8 +3067,11 @@
       <c r="F49">
         <v>555</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>433</v>
       </c>
@@ -2978,7 +3082,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>436</v>
       </c>
@@ -2989,7 +3093,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>439</v>
       </c>
@@ -3000,15 +3104,15 @@
         <v>441</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>7</v>
       </c>
@@ -3024,8 +3128,11 @@
       <c r="F54">
         <v>416</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>14</v>
       </c>
@@ -3510,10 +3617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O291"/>
+  <dimension ref="A1:O304"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="D212" sqref="D212"/>
+    <sheetView tabSelected="1" topLeftCell="B124" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5077,7 +5184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="3" t="s">
         <v>4</v>
       </c>
@@ -5091,7 +5198,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
         <v>4</v>
       </c>
@@ -5105,7 +5212,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
         <v>4</v>
       </c>
@@ -5119,7 +5226,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
         <v>4</v>
       </c>
@@ -5133,7 +5240,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
         <v>4</v>
       </c>
@@ -5147,7 +5254,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
         <v>4</v>
       </c>
@@ -5161,7 +5268,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
         <v>4</v>
       </c>
@@ -5175,7 +5282,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
         <v>4</v>
       </c>
@@ -5189,7 +5296,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
         <v>4</v>
       </c>
@@ -5203,7 +5310,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">
         <v>4</v>
       </c>
@@ -5217,7 +5324,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
         <v>4</v>
       </c>
@@ -5231,7 +5338,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
         <v>4</v>
       </c>
@@ -5245,503 +5352,474 @@
         <v>32</v>
       </c>
     </row>
-    <row r="125" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="J125" s="7"/>
-    </row>
-    <row r="126" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125" s="15">
+        <v>272538750202</v>
+      </c>
+      <c r="D125" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="H126" t="s">
-        <v>556</v>
-      </c>
-      <c r="I126">
-        <v>440</v>
-      </c>
-      <c r="J126" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="K126" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="127" spans="2:11" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C126" s="15">
+        <v>272538750302</v>
+      </c>
+      <c r="D126" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="H127" t="s">
-        <v>556</v>
-      </c>
-      <c r="I127">
-        <v>440</v>
-      </c>
-      <c r="J127" s="6" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="128" spans="2:11" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C127" s="15">
+        <v>272538750303</v>
+      </c>
+      <c r="D127" s="17" t="s">
+        <v>622</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="H128" t="s">
-        <v>556</v>
-      </c>
-      <c r="I128">
-        <v>440</v>
-      </c>
-      <c r="J128" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="K128" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="129" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="5"/>
-      <c r="C129" s="5"/>
-      <c r="D129" s="5"/>
-      <c r="J129" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="C128" s="15">
+        <v>272538750305</v>
+      </c>
+      <c r="D128" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B129" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C129" s="15">
+        <v>272538750406</v>
+      </c>
+      <c r="D129" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="130" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="H130" t="s">
-        <v>556</v>
-      </c>
-      <c r="I130">
-        <v>440</v>
-      </c>
-      <c r="J130" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="K130" t="s">
-        <v>589</v>
+        <v>4</v>
+      </c>
+      <c r="C130" s="15">
+        <v>272538750801</v>
+      </c>
+      <c r="D130" s="17" t="s">
+        <v>623</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="131" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="H131" t="s">
-        <v>556</v>
-      </c>
-      <c r="I131">
-        <v>440</v>
-      </c>
-      <c r="J131" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="K131" t="s">
-        <v>590</v>
+        <v>4</v>
+      </c>
+      <c r="C131" s="15">
+        <v>272538751306</v>
+      </c>
+      <c r="D131" s="17" t="s">
+        <v>624</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="H132" t="s">
-        <v>556</v>
-      </c>
-      <c r="I132">
-        <v>440</v>
-      </c>
-      <c r="J132" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="K132" t="s">
-        <v>591</v>
+        <v>4</v>
+      </c>
+      <c r="C132" s="15">
+        <v>272538753508</v>
+      </c>
+      <c r="D132" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="E132" s="16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="H133" t="s">
-        <v>556</v>
-      </c>
-      <c r="I133">
-        <v>440</v>
-      </c>
-      <c r="J133" s="6" t="s">
-        <v>592</v>
-      </c>
-      <c r="K133" t="s">
-        <v>593</v>
+        <v>4</v>
+      </c>
+      <c r="C133" s="15">
+        <v>272538754112</v>
+      </c>
+      <c r="D133" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="134" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="H134" t="s">
-        <v>556</v>
-      </c>
-      <c r="I134">
-        <v>440</v>
-      </c>
-      <c r="J134" s="6" t="s">
-        <v>594</v>
-      </c>
-      <c r="K134" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="135" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="5"/>
-      <c r="C135" s="5"/>
-      <c r="D135" s="5"/>
-      <c r="J135" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="C134" s="15">
+        <v>272538754114</v>
+      </c>
+      <c r="D134" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="135" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B135" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" s="15">
+        <v>272538755302</v>
+      </c>
+      <c r="D135" s="17" t="s">
+        <v>626</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="136" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>473</v>
+        <v>4</v>
+      </c>
+      <c r="C136" s="15">
+        <v>272538755403</v>
+      </c>
+      <c r="D136" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="E136" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="137" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="138" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="5"/>
-      <c r="C138" s="5"/>
-      <c r="D138" s="5"/>
-      <c r="J138" s="7"/>
-    </row>
-    <row r="139" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B139" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="H139" t="s">
-        <v>560</v>
-      </c>
-      <c r="I139">
-        <v>559</v>
-      </c>
-      <c r="J139" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K139" s="6" t="s">
-        <v>279</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C137" s="15">
+        <v>272538755602</v>
+      </c>
+      <c r="D137" s="17" t="s">
+        <v>628</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="138" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B138" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C138" s="15">
+        <v>272538756805</v>
+      </c>
+      <c r="D138" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="E138" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="139" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="J139" s="7"/>
     </row>
     <row r="140" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="C140" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H140" t="s">
+        <v>556</v>
+      </c>
+      <c r="I140">
+        <v>440</v>
+      </c>
+      <c r="J140" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="K140" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="141" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B141" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C141" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D140" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="H140" t="s">
-        <v>560</v>
-      </c>
-      <c r="I140">
-        <v>559</v>
-      </c>
-      <c r="J140" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K140" s="6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="141" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="5"/>
-      <c r="C141" s="5"/>
-      <c r="D141" s="5"/>
-      <c r="J141" s="7"/>
+      <c r="D141" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="H141" t="s">
+        <v>556</v>
+      </c>
+      <c r="I141">
+        <v>440</v>
+      </c>
+      <c r="J141" s="6" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="142" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H142" t="s">
-        <v>17</v>
+        <v>556</v>
       </c>
       <c r="I142">
-        <v>556</v>
+        <v>440</v>
       </c>
       <c r="J142" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K142" s="6" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="143" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B143" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="H143" t="s">
-        <v>17</v>
-      </c>
-      <c r="I143">
-        <v>556</v>
-      </c>
-      <c r="J143" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K143" s="6" t="s">
-        <v>275</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="K142" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="143" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="J143" s="7"/>
     </row>
     <row r="144" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>142</v>
+        <v>466</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H144" t="s">
-        <v>17</v>
+        <v>556</v>
       </c>
       <c r="I144">
+        <v>440</v>
+      </c>
+      <c r="J144" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="K144" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="145" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B145" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H145" t="s">
         <v>556</v>
       </c>
-      <c r="J144" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K144" s="6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="145" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="5"/>
-      <c r="C145" s="5"/>
-      <c r="D145" s="5"/>
-      <c r="J145" s="7"/>
+      <c r="I145">
+        <v>440</v>
+      </c>
+      <c r="J145" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="K145" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="146" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>140</v>
+        <v>468</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H146" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I146">
-        <v>557</v>
+        <v>440</v>
       </c>
       <c r="J146" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K146" s="6" t="s">
-        <v>277</v>
+        <v>513</v>
+      </c>
+      <c r="K146" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="147" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>141</v>
+        <v>469</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>278</v>
+        <v>470</v>
       </c>
       <c r="H147" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I147">
-        <v>557</v>
+        <v>440</v>
       </c>
       <c r="J147" s="6" t="s">
-        <v>598</v>
-      </c>
-      <c r="K147" s="6" t="s">
-        <v>599</v>
+        <v>591</v>
+      </c>
+      <c r="K147" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="148" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="C148" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D148" s="6"/>
-      <c r="K148" s="6"/>
+        <v>465</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="H148" t="s">
+        <v>556</v>
+      </c>
+      <c r="I148">
+        <v>440</v>
+      </c>
+      <c r="J148" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="K148" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="149" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
       <c r="J149" s="7"/>
     </row>
     <row r="150" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="H150" t="s">
-        <v>558</v>
-      </c>
-      <c r="I150">
-        <v>410</v>
+        <v>473</v>
       </c>
     </row>
     <row r="151" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="H151" t="s">
-        <v>558</v>
-      </c>
-      <c r="I151">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="152" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B152" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D152" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="H152" t="s">
-        <v>558</v>
-      </c>
-      <c r="I152">
-        <v>410</v>
-      </c>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="152" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+      <c r="J152" s="7"/>
     </row>
     <row r="153" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>482</v>
+        <v>279</v>
       </c>
       <c r="H153" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="I153">
-        <v>410</v>
+        <v>559</v>
+      </c>
+      <c r="J153" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K153" s="6" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="154" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>483</v>
+        <v>280</v>
       </c>
       <c r="H154" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="I154">
-        <v>410</v>
+        <v>559</v>
+      </c>
+      <c r="J154" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K154" s="6" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="155" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5752,1875 +5830,2081 @@
     </row>
     <row r="156" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B156" s="3" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="H156" t="s">
-        <v>559</v>
+        <v>17</v>
       </c>
       <c r="I156">
-        <v>411</v>
+        <v>556</v>
       </c>
       <c r="J156" s="6" t="s">
         <v>140</v>
       </c>
       <c r="K156" s="6" t="s">
-        <v>576</v>
+        <v>274</v>
       </c>
     </row>
     <row r="157" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="H157" t="s">
-        <v>559</v>
+        <v>17</v>
       </c>
       <c r="I157">
-        <v>411</v>
+        <v>556</v>
       </c>
       <c r="J157" s="6" t="s">
-        <v>600</v>
+        <v>141</v>
       </c>
       <c r="K157" s="6" t="s">
-        <v>601</v>
+        <v>275</v>
       </c>
     </row>
     <row r="158" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B158" s="3" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>142</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>485</v>
+        <v>276</v>
       </c>
       <c r="H158" t="s">
-        <v>559</v>
+        <v>17</v>
       </c>
       <c r="I158">
-        <v>411</v>
+        <v>556</v>
       </c>
       <c r="J158" s="6" t="s">
         <v>142</v>
       </c>
       <c r="K158" s="6" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="159" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B159" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="H159" t="s">
-        <v>559</v>
-      </c>
-      <c r="I159">
-        <v>411</v>
-      </c>
-      <c r="J159" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="K159" s="6" t="s">
-        <v>486</v>
-      </c>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="159" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="5"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+      <c r="J159" s="7"/>
     </row>
     <row r="160" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H160" t="s">
+        <v>557</v>
+      </c>
+      <c r="I160">
+        <v>557</v>
+      </c>
+      <c r="J160" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K160" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B161" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H161" t="s">
+        <v>557</v>
+      </c>
+      <c r="I161">
+        <v>557</v>
+      </c>
+      <c r="J161" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="K161" s="6" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B162" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C162" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D162" s="6"/>
+      <c r="K162" s="6"/>
+    </row>
+    <row r="163" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J163" s="7"/>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B164" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="H164" t="s">
+        <v>558</v>
+      </c>
+      <c r="I164">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B165" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="H165" t="s">
+        <v>558</v>
+      </c>
+      <c r="I165">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B166" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="H166" t="s">
+        <v>558</v>
+      </c>
+      <c r="I166">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B167" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="H167" t="s">
+        <v>558</v>
+      </c>
+      <c r="I167">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B168" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="H168" t="s">
+        <v>558</v>
+      </c>
+      <c r="I168">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B169" s="5"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+      <c r="J169" s="7"/>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B170" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="C170" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H170" t="s">
+        <v>559</v>
+      </c>
+      <c r="I170">
+        <v>411</v>
+      </c>
+      <c r="J170" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K170" s="6" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B171" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H171" t="s">
+        <v>559</v>
+      </c>
+      <c r="I171">
+        <v>411</v>
+      </c>
+      <c r="J171" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="K171" s="6" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B172" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="H172" t="s">
+        <v>559</v>
+      </c>
+      <c r="I172">
+        <v>411</v>
+      </c>
+      <c r="J172" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K172" s="6" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B173" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="H173" t="s">
+        <v>559</v>
+      </c>
+      <c r="I173">
+        <v>411</v>
+      </c>
+      <c r="J173" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="K173" s="6" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B174" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C174" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="D174" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H160" t="s">
+      <c r="H174" t="s">
         <v>559</v>
       </c>
-      <c r="I160">
+      <c r="I174">
         <v>411</v>
       </c>
-      <c r="J160" s="6" t="s">
+      <c r="J174" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="K160" s="6" t="s">
+      <c r="K174" s="6" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B161" s="3" t="s">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B175" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="C161" s="3" t="s">
+      <c r="C175" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D175" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="H161" t="s">
+      <c r="H175" t="s">
         <v>559</v>
       </c>
-      <c r="I161">
+      <c r="I175">
         <v>411</v>
       </c>
-      <c r="J161" s="6" t="s">
+      <c r="J175" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="K161" s="6" t="s">
+      <c r="K175" s="6" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="162" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="10"/>
-      <c r="B162" s="8" t="s">
+    <row r="176" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="10"/>
+      <c r="B176" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="C162" s="8" t="s">
+      <c r="C176" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D162" s="8" t="s">
+      <c r="D176" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="G162" s="12"/>
-      <c r="J162" s="13"/>
-      <c r="K162" s="13"/>
-    </row>
-    <row r="163" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="10"/>
-      <c r="B163" s="8"/>
-      <c r="C163" s="8"/>
-      <c r="D163" s="8"/>
-      <c r="G163" s="12"/>
-      <c r="J163" s="13"/>
-      <c r="K163" s="13"/>
-    </row>
-    <row r="164" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="5"/>
-      <c r="C164" s="5"/>
-      <c r="D164" s="5"/>
-      <c r="J164" s="7"/>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B165" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D165" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="H165" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="I165" s="11">
-        <v>439</v>
-      </c>
-      <c r="J165" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K165" s="6" t="s">
-        <v>578</v>
-      </c>
-      <c r="L165" s="13"/>
-      <c r="M165" s="13"/>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B166" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="H166" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="I166" s="11">
-        <v>439</v>
-      </c>
-      <c r="J166" s="6" t="s">
-        <v>596</v>
-      </c>
-      <c r="K166" s="6" t="s">
-        <v>597</v>
-      </c>
-      <c r="L166" s="13"/>
-      <c r="M166" s="13"/>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B167" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D167" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H167" t="s">
-        <v>570</v>
-      </c>
-      <c r="I167">
-        <v>439</v>
-      </c>
-      <c r="J167" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K167" s="6" t="s">
-        <v>577</v>
-      </c>
-      <c r="L167" s="6"/>
-      <c r="M167" s="6"/>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B168" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D168" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="H168" t="s">
-        <v>570</v>
-      </c>
-      <c r="I168">
-        <v>439</v>
-      </c>
-      <c r="J168" s="6" t="s">
-        <v>602</v>
-      </c>
-      <c r="K168" s="6" t="s">
-        <v>603</v>
-      </c>
-      <c r="L168" s="6"/>
-      <c r="M168" s="6"/>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B169" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D169" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="H169" t="s">
-        <v>570</v>
-      </c>
-      <c r="I169">
-        <v>439</v>
-      </c>
-      <c r="J169" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="K169" s="6" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B170" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="H170" t="s">
-        <v>570</v>
-      </c>
-      <c r="I170">
-        <v>439</v>
-      </c>
-      <c r="J170" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="K170" s="6" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H171" s="11"/>
-      <c r="I171" s="11"/>
-      <c r="L171" s="13"/>
-      <c r="M171" s="13"/>
-    </row>
-    <row r="172" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J172" s="7"/>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B173" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D173" s="3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B174" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D174" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B175" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B176" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D176" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="177" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B177" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D177" s="3" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="178" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G176" s="12"/>
+      <c r="J176" s="13"/>
+      <c r="K176" s="13"/>
+    </row>
+    <row r="177" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="10"/>
+      <c r="B177" s="8"/>
+      <c r="C177" s="8"/>
+      <c r="D177" s="8"/>
+      <c r="G177" s="12"/>
+      <c r="J177" s="13"/>
+      <c r="K177" s="13"/>
+    </row>
+    <row r="178" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
       <c r="J178" s="7"/>
     </row>
-    <row r="179" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B179" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="180" spans="2:10" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="H179" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="I179" s="11">
+        <v>439</v>
+      </c>
+      <c r="J179" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K179" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="L179" s="13"/>
+      <c r="M179" s="13"/>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="181" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B181" s="5"/>
-      <c r="C181" s="5"/>
-      <c r="D181" s="5"/>
-      <c r="J181" s="7"/>
-    </row>
-    <row r="182" spans="2:10" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="H180" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="I180" s="11">
+        <v>439</v>
+      </c>
+      <c r="J180" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="K180" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="L180" s="13"/>
+      <c r="M180" s="13"/>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B181" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H181" t="s">
+        <v>570</v>
+      </c>
+      <c r="I181">
+        <v>439</v>
+      </c>
+      <c r="J181" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K181" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="L181" s="6"/>
+      <c r="M181" s="6"/>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B182" s="3" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="183" spans="2:10" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="H182" t="s">
+        <v>570</v>
+      </c>
+      <c r="I182">
+        <v>439</v>
+      </c>
+      <c r="J182" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="K182" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="L182" s="6"/>
+      <c r="M182" s="6"/>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B183" s="3" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="184" spans="2:10" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="H183" t="s">
+        <v>570</v>
+      </c>
+      <c r="I183">
+        <v>439</v>
+      </c>
+      <c r="J183" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="K183" s="6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="185" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B185" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D185" s="3" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="186" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="5"/>
-      <c r="C186" s="5"/>
-      <c r="D186" s="5"/>
+        <v>301</v>
+      </c>
+      <c r="H184" t="s">
+        <v>570</v>
+      </c>
+      <c r="I184">
+        <v>439</v>
+      </c>
+      <c r="J184" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="K184" s="6" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H185" s="11"/>
+      <c r="I185" s="11"/>
+      <c r="L185" s="13"/>
+      <c r="M185" s="13"/>
+    </row>
+    <row r="186" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J186" s="7"/>
     </row>
-    <row r="187" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B187" s="3" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="188" spans="2:10" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="189" spans="2:10" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>142</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="190" spans="2:10" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>143</v>
       </c>
       <c r="D190" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B191" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B192" s="5"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="5"/>
+      <c r="J192" s="7"/>
+    </row>
+    <row r="193" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B193" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="194" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B194" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="195" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B195" s="5"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="5"/>
+      <c r="J195" s="7"/>
+    </row>
+    <row r="196" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B196" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="197" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B197" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="198" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B198" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="199" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B199" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="200" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B200" s="5"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="5"/>
+      <c r="J200" s="7"/>
+    </row>
+    <row r="201" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B201" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="202" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B202" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="203" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B203" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="204" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B204" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D204" s="3" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="191" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="5"/>
-      <c r="C191" s="5"/>
-      <c r="D191" s="5"/>
-      <c r="J191" s="7"/>
-    </row>
-    <row r="192" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B192" s="3" t="s">
+    <row r="205" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B205" s="5"/>
+      <c r="C205" s="5"/>
+      <c r="D205" s="5"/>
+      <c r="J205" s="7"/>
+    </row>
+    <row r="206" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B206" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="C192" s="3" t="s">
+      <c r="C206" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D192" s="3" t="s">
+      <c r="D206" s="3" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B193" s="3" t="s">
+    <row r="207" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B207" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="C193" s="3" t="s">
+      <c r="C207" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D193" s="3" t="s">
+      <c r="D207" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B194" s="3" t="s">
+    <row r="208" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B208" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="C194" s="3" t="s">
+      <c r="C208" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D194" s="3" t="s">
+      <c r="D208" s="3" t="s">
         <v>318</v>
-      </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B195" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B196" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D196" s="3" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="197" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="5"/>
-      <c r="C197" s="5"/>
-      <c r="D197" s="5"/>
-      <c r="J197" s="7"/>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B198" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D198" s="3" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B199" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D199" s="3" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B200" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D200" s="3" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B201" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D201" s="3" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="202" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="5"/>
-      <c r="C202" s="5"/>
-      <c r="D202" s="5"/>
-      <c r="J202" s="7"/>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="C203" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D203" s="3" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B204" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D204" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B205" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D205" s="3" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B206" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D206" s="3" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="207" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="5"/>
-      <c r="C207" s="5"/>
-      <c r="D207" s="5"/>
-      <c r="J207" s="7"/>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A208" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D208" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G208" s="2" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="F209" s="3" t="s">
-        <v>512</v>
+        <v>319</v>
       </c>
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="F210" s="3" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B211" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D211" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="G211" s="2" t="s">
-        <v>608</v>
-      </c>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B211" s="5"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="5"/>
+      <c r="J211" s="7"/>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="C212" s="14">
-        <v>13</v>
+        <v>503</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="213" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B213" s="5"/>
-      <c r="C213" s="5"/>
-      <c r="D213" s="5"/>
-      <c r="J213" s="7"/>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B213" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A214" s="1" t="s">
-        <v>405</v>
-      </c>
       <c r="B214" s="3" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>516</v>
+        <v>142</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="G214" s="2" t="s">
-        <v>605</v>
+        <v>506</v>
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>518</v>
+        <v>143</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="G215" s="2" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B216" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="D216" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G216" s="2" t="s">
-        <v>607</v>
-      </c>
+        <v>507</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B216" s="5"/>
+      <c r="C216" s="5"/>
+      <c r="D216" s="5"/>
+      <c r="J216" s="7"/>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>399</v>
+      </c>
       <c r="B217" s="3" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>520</v>
+        <v>140</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="G217" s="2" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="218" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B218" s="5"/>
-      <c r="C218" s="5"/>
-      <c r="D218" s="5"/>
-      <c r="J218" s="7"/>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B218" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A219" s="1" t="s">
-        <v>408</v>
-      </c>
       <c r="B219" s="3" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>516</v>
+        <v>142</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B221" s="5"/>
+      <c r="C221" s="5"/>
+      <c r="D221" s="5"/>
+      <c r="J221" s="7"/>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G222" s="2" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B223" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="F223" s="3" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B224" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="F224" s="3" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B225" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="G225" s="2" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B226" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C226" s="14">
+        <v>13</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B227" s="5"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="5"/>
+      <c r="J227" s="7"/>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C228" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="G228" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B229" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G229" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B230" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="G230" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B231" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="G231" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B232" s="5"/>
+      <c r="C232" s="5"/>
+      <c r="D232" s="5"/>
+      <c r="J232" s="7"/>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B233" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="C220" s="3" t="s">
+      <c r="C233" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B234" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C234" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="D220" s="3" t="s">
+      <c r="D234" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B221" s="3" t="s">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B235" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="C221" s="3" t="s">
+      <c r="C235" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="D221" s="3" t="s">
+      <c r="D235" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B222" s="3" t="s">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B236" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="C222" s="3" t="s">
+      <c r="C236" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="D222" s="3" t="s">
+      <c r="D236" s="3" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="223" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="5"/>
-      <c r="C223" s="5"/>
-      <c r="D223" s="5"/>
-      <c r="J223" s="7"/>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A224" s="1" t="s">
+    <row r="237" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B237" s="5"/>
+      <c r="C237" s="5"/>
+      <c r="D237" s="5"/>
+      <c r="J237" s="7"/>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B224" s="3" t="s">
+      <c r="B238" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="C224" s="3" t="s">
+      <c r="C238" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="D224" s="3" t="s">
+      <c r="D238" s="3" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="225" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B225" s="3" t="s">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B239" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="C225" s="3" t="s">
+      <c r="C239" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="D225" s="3" t="s">
+      <c r="D239" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="226" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B226" s="3" t="s">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B240" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="C226" s="3" t="s">
+      <c r="C240" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="D226" s="3" t="s">
+      <c r="D240" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="227" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B227" s="3" t="s">
+    <row r="241" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B241" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="C227" s="3" t="s">
+      <c r="C241" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="D227" s="3" t="s">
+      <c r="D241" s="3" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="228" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B228" s="5"/>
-      <c r="C228" s="5"/>
-      <c r="D228" s="5"/>
-      <c r="J228" s="7"/>
-    </row>
-    <row r="229" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B229" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="C229" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D229" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="K229" s="6"/>
-    </row>
-    <row r="230" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B230" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D230" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="K230" s="6"/>
-    </row>
-    <row r="231" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B231" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D231" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="K231" s="6"/>
-    </row>
-    <row r="232" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B232" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="C232" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D232" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="K232" s="6"/>
-    </row>
-    <row r="233" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K233" s="6"/>
-    </row>
-    <row r="234" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J234" s="7"/>
-    </row>
-    <row r="235" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B235" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="H235" t="s">
-        <v>566</v>
-      </c>
-      <c r="I235">
-        <v>441</v>
-      </c>
-      <c r="J235" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K235" s="6" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="236" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B236" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="C236" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="G236" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="H236" t="s">
-        <v>566</v>
-      </c>
-      <c r="I236">
-        <v>441</v>
-      </c>
-      <c r="J236" s="6" t="s">
-        <v>600</v>
-      </c>
-      <c r="K236" s="6" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="237" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B237" s="3"/>
-      <c r="C237" s="3"/>
-      <c r="D237" s="3"/>
-      <c r="K237" s="6"/>
-    </row>
-    <row r="238" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B238" s="5"/>
-      <c r="C238" s="5"/>
-      <c r="D238" s="5"/>
-      <c r="J238" s="7"/>
-    </row>
-    <row r="239" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B239" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D239" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H239" t="s">
-        <v>595</v>
-      </c>
-      <c r="I239">
-        <v>455</v>
-      </c>
-      <c r="J239" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="K239" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="240" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B240" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="C240" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D240" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="H240" t="s">
-        <v>595</v>
-      </c>
-      <c r="I240">
-        <v>455</v>
-      </c>
-      <c r="J240" s="6" t="s">
-        <v>614</v>
-      </c>
-      <c r="K240" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="241" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J241"/>
-    </row>
-    <row r="242" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B242" s="5"/>
+      <c r="C242" s="5"/>
+      <c r="D242" s="5"/>
+      <c r="J242" s="7"/>
+    </row>
     <row r="243" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>493</v>
-      </c>
+        <v>524</v>
+      </c>
+      <c r="K243" s="6"/>
     </row>
     <row r="244" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>494</v>
-      </c>
+        <v>525</v>
+      </c>
+      <c r="K244" s="6"/>
     </row>
     <row r="245" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>142</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="246" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="5"/>
-      <c r="C246" s="5"/>
-      <c r="D246" s="5"/>
-      <c r="J246" s="7"/>
+        <v>526</v>
+      </c>
+      <c r="K245" s="6"/>
+    </row>
+    <row r="246" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B246" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="K246" s="6"/>
     </row>
     <row r="247" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B247" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D247" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="H247" t="s">
-        <v>567</v>
-      </c>
-      <c r="I247">
-        <v>443</v>
-      </c>
-      <c r="J247" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K247" s="6" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="248" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B248" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="C248" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D248" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="H248" t="s">
-        <v>567</v>
-      </c>
-      <c r="I248">
-        <v>443</v>
-      </c>
-      <c r="J248" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K248" s="6" t="s">
-        <v>582</v>
-      </c>
+      <c r="K247" s="6"/>
+    </row>
+    <row r="248" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J248" s="7"/>
     </row>
     <row r="249" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="H249" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I249">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J249" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K249" s="6" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
     </row>
     <row r="250" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B250" s="3" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>303</v>
+        <v>280</v>
+      </c>
+      <c r="G250" s="2" t="s">
+        <v>615</v>
       </c>
       <c r="H250" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I250">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J250" s="6" t="s">
-        <v>143</v>
+        <v>599</v>
       </c>
       <c r="K250" s="6" t="s">
-        <v>303</v>
+        <v>612</v>
       </c>
     </row>
     <row r="251" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B251" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="C251" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D251" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="H251" t="s">
-        <v>567</v>
-      </c>
-      <c r="I251">
-        <v>443</v>
-      </c>
-      <c r="J251" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="K251" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="252" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B252" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="C252" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D252" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="H252" t="s">
-        <v>567</v>
-      </c>
-      <c r="I252">
-        <v>443</v>
-      </c>
-      <c r="J252" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K252" s="6" t="s">
-        <v>583</v>
-      </c>
+      <c r="B251" s="3"/>
+      <c r="C251" s="3"/>
+      <c r="D251" s="3"/>
+      <c r="K251" s="6"/>
+    </row>
+    <row r="252" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B252" s="5"/>
+      <c r="C252" s="5"/>
+      <c r="D252" s="5"/>
+      <c r="J252" s="7"/>
     </row>
     <row r="253" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B253" s="3" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="H253" t="s">
-        <v>567</v>
+        <v>594</v>
       </c>
       <c r="I253">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="J253" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="K253" s="6" t="s">
-        <v>306</v>
+        <v>316</v>
+      </c>
+      <c r="K253" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="254" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B254" s="3" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>307</v>
+        <v>530</v>
       </c>
       <c r="H254" t="s">
-        <v>567</v>
+        <v>594</v>
       </c>
       <c r="I254">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="J254" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="K254" s="6" t="s">
-        <v>324</v>
+        <v>613</v>
+      </c>
+      <c r="K254" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="255" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K255" s="6"/>
-    </row>
-    <row r="256" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J256" s="7"/>
-    </row>
+      <c r="J255"/>
+    </row>
+    <row r="256" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="257" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B257" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="H257" t="s">
-        <v>568</v>
-      </c>
-      <c r="I257">
-        <v>442</v>
-      </c>
-      <c r="J257" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K257" s="6" t="s">
-        <v>308</v>
+        <v>493</v>
       </c>
     </row>
     <row r="258" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B258" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="H258" t="s">
-        <v>568</v>
-      </c>
-      <c r="I258">
-        <v>442</v>
-      </c>
-      <c r="J258" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="K258" s="6" t="s">
-        <v>309</v>
+        <v>494</v>
       </c>
     </row>
     <row r="259" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B259" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>142</v>
       </c>
       <c r="D259" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="H259" t="s">
-        <v>568</v>
-      </c>
-      <c r="I259">
-        <v>442</v>
-      </c>
-      <c r="J259" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K259" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="260" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B260" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="C260" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D260" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="H260" t="s">
-        <v>568</v>
-      </c>
-      <c r="I260">
-        <v>442</v>
-      </c>
-      <c r="J260" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="K260" s="6" t="s">
-        <v>311</v>
-      </c>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="260" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B260" s="5"/>
+      <c r="C260" s="5"/>
+      <c r="D260" s="5"/>
+      <c r="J260" s="7"/>
     </row>
     <row r="261" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B261" s="3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="H261" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I261">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J261" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K261" s="6" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="262" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B262" s="3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>312</v>
+        <v>535</v>
       </c>
       <c r="H262" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I262">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J262" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K262" s="6" t="s">
-        <v>312</v>
+        <v>581</v>
       </c>
     </row>
     <row r="263" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B263" s="3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="H263" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I263">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J263" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K263" s="6" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="264" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B264" s="3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H264" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I264">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J264" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K264" s="6" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="265" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K265" s="6"/>
-    </row>
-    <row r="266" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J266" s="7"/>
+      <c r="B265" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D265" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="H265" t="s">
+        <v>567</v>
+      </c>
+      <c r="I265">
+        <v>443</v>
+      </c>
+      <c r="J265" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="K265" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="266" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B266" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D266" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="H266" t="s">
+        <v>567</v>
+      </c>
+      <c r="I266">
+        <v>443</v>
+      </c>
+      <c r="J266" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K266" s="6" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="267" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B267" s="3" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>287</v>
+        <v>306</v>
       </c>
       <c r="H267" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="I267">
-        <v>555</v>
+        <v>443</v>
       </c>
       <c r="J267" s="6" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="K267" s="6" t="s">
-        <v>287</v>
+        <v>306</v>
       </c>
     </row>
     <row r="268" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B268" s="3" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>288</v>
+        <v>307</v>
       </c>
       <c r="H268" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="I268">
-        <v>555</v>
+        <v>443</v>
       </c>
       <c r="J268" s="6" t="s">
-        <v>141</v>
+        <v>620</v>
       </c>
       <c r="K268" s="6" t="s">
-        <v>288</v>
+        <v>324</v>
       </c>
     </row>
     <row r="269" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B269" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="C269" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D269" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="H269" t="s">
-        <v>569</v>
-      </c>
-      <c r="I269">
-        <v>555</v>
-      </c>
-      <c r="J269" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K269" s="6" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="270" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B270" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="C270" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D270" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="H270" t="s">
-        <v>569</v>
-      </c>
-      <c r="I270">
-        <v>555</v>
-      </c>
-      <c r="J270" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="K270" s="6" t="s">
-        <v>290</v>
-      </c>
+      <c r="K269" s="6"/>
+    </row>
+    <row r="270" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J270" s="7"/>
     </row>
     <row r="271" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B271" s="3" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>539</v>
+        <v>308</v>
       </c>
       <c r="H271" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I271">
-        <v>555</v>
+        <v>442</v>
       </c>
       <c r="J271" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K271" s="6" t="s">
-        <v>539</v>
+        <v>308</v>
       </c>
     </row>
     <row r="272" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B272" s="3" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>540</v>
+        <v>309</v>
       </c>
       <c r="H272" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I272">
-        <v>555</v>
+        <v>442</v>
       </c>
       <c r="J272" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K272" s="6" t="s">
-        <v>585</v>
+        <v>309</v>
       </c>
     </row>
     <row r="273" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B273" s="3" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>541</v>
+        <v>310</v>
       </c>
       <c r="H273" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I273">
-        <v>555</v>
-      </c>
-      <c r="K273" s="7"/>
+        <v>442</v>
+      </c>
+      <c r="J273" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K273" s="6" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="274" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B274" s="3" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="H274" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I274">
-        <v>555</v>
+        <v>442</v>
       </c>
       <c r="J274" s="6" t="s">
-        <v>616</v>
+        <v>143</v>
       </c>
       <c r="K274" s="6" t="s">
-        <v>617</v>
+        <v>311</v>
       </c>
     </row>
     <row r="275" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B275" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="C275" s="14" t="s">
-        <v>516</v>
+        <v>536</v>
+      </c>
+      <c r="C275" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D275" s="3" t="s">
+        <v>537</v>
       </c>
       <c r="H275" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I275">
-        <v>555</v>
+        <v>442</v>
       </c>
       <c r="J275" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K275" s="6" t="s">
-        <v>574</v>
+        <v>583</v>
       </c>
     </row>
     <row r="276" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B276" s="3"/>
-      <c r="C276" s="14"/>
-      <c r="K276" s="6"/>
-    </row>
-    <row r="277" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J277" s="7"/>
+      <c r="B276" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C276" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D276" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H276" t="s">
+        <v>568</v>
+      </c>
+      <c r="I276">
+        <v>442</v>
+      </c>
+      <c r="J276" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K276" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="277" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B277" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D277" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="H277" t="s">
+        <v>568</v>
+      </c>
+      <c r="I277">
+        <v>442</v>
+      </c>
+      <c r="J277" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="K277" s="6" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="278" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B278" s="3" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>543</v>
+        <v>307</v>
+      </c>
+      <c r="H278" t="s">
+        <v>568</v>
+      </c>
+      <c r="I278">
+        <v>442</v>
+      </c>
+      <c r="J278" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="K278" s="6" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="279" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B279" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="C279" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D279" s="3" t="s">
-        <v>544</v>
-      </c>
+      <c r="K279" s="6"/>
     </row>
     <row r="280" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B280" s="5"/>
-      <c r="C280" s="5"/>
-      <c r="D280" s="5"/>
       <c r="J280" s="7"/>
     </row>
     <row r="281" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B281" s="3" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C281" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>546</v>
+        <v>287</v>
+      </c>
+      <c r="H281" t="s">
+        <v>569</v>
+      </c>
+      <c r="I281">
+        <v>555</v>
+      </c>
+      <c r="J281" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K281" s="6" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="282" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B282" s="3" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>547</v>
+        <v>288</v>
+      </c>
+      <c r="H282" t="s">
+        <v>569</v>
+      </c>
+      <c r="I282">
+        <v>555</v>
+      </c>
+      <c r="J282" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K282" s="6" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="283" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B283" s="3" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>142</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>548</v>
+        <v>289</v>
+      </c>
+      <c r="H283" t="s">
+        <v>569</v>
+      </c>
+      <c r="I283">
+        <v>555</v>
+      </c>
+      <c r="J283" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K283" s="6" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="284" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B284" s="3" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>143</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>549</v>
+        <v>290</v>
+      </c>
+      <c r="H284" t="s">
+        <v>569</v>
+      </c>
+      <c r="I284">
+        <v>555</v>
+      </c>
+      <c r="J284" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="K284" s="6" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="285" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B285" s="3" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="286" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B286" s="5"/>
-      <c r="C286" s="5"/>
-      <c r="D286" s="5"/>
-      <c r="J286" s="7"/>
+        <v>539</v>
+      </c>
+      <c r="H285" t="s">
+        <v>569</v>
+      </c>
+      <c r="I285">
+        <v>555</v>
+      </c>
+      <c r="J285" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="K285" s="6" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="286" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B286" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="C286" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="H286" t="s">
+        <v>569</v>
+      </c>
+      <c r="I286">
+        <v>555</v>
+      </c>
+      <c r="J286" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K286" s="6" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="287" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B287" s="3" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>284</v>
-      </c>
+        <v>541</v>
+      </c>
+      <c r="H287" t="s">
+        <v>569</v>
+      </c>
+      <c r="I287">
+        <v>555</v>
+      </c>
+      <c r="K287" s="7"/>
     </row>
     <row r="288" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B288" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="C288" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D288" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="H288" t="s">
+        <v>569</v>
+      </c>
+      <c r="I288">
+        <v>555</v>
+      </c>
+      <c r="J288" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="K288" s="6" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="289" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B289" s="3"/>
+      <c r="C289" s="14"/>
+      <c r="K289" s="6"/>
+    </row>
+    <row r="290" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J290" s="7"/>
+    </row>
+    <row r="291" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B291" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D291" s="3" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="292" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B292" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="C292" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D292" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="293" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B293" s="5"/>
+      <c r="C293" s="5"/>
+      <c r="D293" s="5"/>
+      <c r="J293" s="7"/>
+    </row>
+    <row r="294" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B294" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C294" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D294" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="295" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B295" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C295" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D295" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="296" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B296" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="297" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B297" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D297" s="3" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="298" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B298" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C298" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D298" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="299" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B299" s="5"/>
+      <c r="C299" s="5"/>
+      <c r="D299" s="5"/>
+      <c r="J299" s="7"/>
+    </row>
+    <row r="300" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B300" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="C288" s="3" t="s">
+      <c r="C300" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D300" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="301" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B301" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="C301" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D288" s="3" t="s">
+      <c r="D301" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="F288" s="3" t="s">
+      <c r="F301" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="289" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B289" s="3" t="s">
+    <row r="302" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B302" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="C289" s="3" t="s">
+      <c r="C302" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D289" s="3" t="s">
+      <c r="D302" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="F289" s="3" t="s">
+      <c r="F302" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="290" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B290" s="3" t="s">
+    <row r="303" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B303" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="C290" s="3" t="s">
+      <c r="C303" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D290" s="3" t="s">
+      <c r="D303" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="F290" s="3" t="s">
+      <c r="F303" s="3" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="291" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B291" s="3" t="s">
+    <row r="304" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B304" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="C291" s="3" t="s">
+      <c r="C304" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D291" s="3" t="s">
+      <c r="D304" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="F291" s="3" t="s">
+      <c r="F304" s="3" t="s">
         <v>512</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>